<commit_message>
Banking app tests completed using wrapper
</commit_message>
<xml_diff>
--- a/techtask/testcases.xlsx
+++ b/techtask/testcases.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -236,7 +237,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -246,6 +247,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -262,13 +269,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -551,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,7 +672,7 @@
       <c r="B15">
         <v>3</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D15" t="s">
@@ -672,7 +680,7 @@
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+      <c r="C16" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D16" t="s">
@@ -680,7 +688,7 @@
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+      <c r="C17" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D17" t="s">
@@ -688,7 +696,7 @@
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+      <c r="C18" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D18" t="s">
@@ -704,7 +712,7 @@
       <c r="B20">
         <v>4</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D20" t="s">
@@ -712,7 +720,7 @@
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
+      <c r="C21" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D21" t="s">
@@ -720,7 +728,7 @@
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
+      <c r="C22" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D22" t="s">
@@ -728,12 +736,13 @@
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C23" s="4"/>
       <c r="D23" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
+      <c r="C24" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D24" t="s">
@@ -741,12 +750,13 @@
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C25" s="4"/>
       <c r="D25" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
+      <c r="C26" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D26" t="s">
@@ -754,6 +764,7 @@
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C27" s="4"/>
       <c r="D27" t="s">
         <v>43</v>
       </c>
@@ -762,7 +773,7 @@
       <c r="B29">
         <v>5</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D29" t="s">
@@ -770,12 +781,12 @@
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
+      <c r="C30" s="4" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
+      <c r="C31" s="4" t="s">
         <v>47</v>
       </c>
       <c r="D31" t="s">
@@ -783,7 +794,7 @@
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
+      <c r="C32" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D32" t="s">
@@ -791,7 +802,7 @@
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
+      <c r="C33" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D33" t="s">
@@ -799,7 +810,7 @@
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
+      <c r="C34" s="4" t="s">
         <v>53</v>
       </c>
       <c r="D34" t="s">
@@ -807,7 +818,7 @@
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
+      <c r="C35" s="4" t="s">
         <v>55</v>
       </c>
       <c r="D35" t="s">
@@ -818,7 +829,7 @@
       <c r="B37">
         <v>6</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="4" t="s">
         <v>57</v>
       </c>
       <c r="D37" t="s">
@@ -826,7 +837,7 @@
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
+      <c r="C38" s="4" t="s">
         <v>59</v>
       </c>
       <c r="D38" t="s">
@@ -834,7 +845,7 @@
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
+      <c r="C39" s="4" t="s">
         <v>61</v>
       </c>
       <c r="D39" t="s">

</xml_diff>

<commit_message>
Experiments with Excel sheet
</commit_message>
<xml_diff>
--- a/techtask/testcases.xlsx
+++ b/techtask/testcases.xlsx
@@ -560,7 +560,7 @@
   <dimension ref="B2:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,12 +781,12 @@
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="3" t="s">
         <v>47</v>
       </c>
       <c r="D31" t="s">
@@ -794,7 +794,7 @@
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D32" t="s">
@@ -802,7 +802,7 @@
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="3" t="s">
         <v>51</v>
       </c>
       <c r="D33" t="s">

</xml_diff>